<commit_message>
Pre-production revision of LAS prints. Includes set of prints and models converted to .dxf/.pdf/.stp for manufacturing use. AA
</commit_message>
<xml_diff>
--- a/solidworks/Line Angle Sensor/LAS BOM.xlsx
+++ b/solidworks/Line Angle Sensor/LAS BOM.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\MHK Model\documentation\kiteCAD\solidworks\Line Angle Sensor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\KiteCAD\kiteCADRepo\solidworks\Line Angle Sensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18CA6946-4C6F-49B0-A462-F55E00D07C0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC84DCA6-42D6-4220-9517-FB5CC55A1E87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="1215" windowWidth="21600" windowHeight="11325" xr2:uid="{55FD3AFF-6DA2-47EA-AB10-38044739AE1F}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="28770" windowHeight="15300" xr2:uid="{57B7DC1C-58AE-4505-9A04-94FF693A4A73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
-    <customWorkbookView name="andre - Personal View" guid="{9D63CC60-58DB-454E-9D11-4AC495F4C5E2}" mergeInterval="0" personalView="1" xWindow="81" yWindow="81" windowWidth="1440" windowHeight="755" activeSheetId="1"/>
+    <customWorkbookView name="andre - Personal View" guid="{638AF512-54A5-44A6-8E4F-2CB6AF9DF51F}" mergeInterval="0" personalView="1" xWindow="1" windowWidth="1918" windowHeight="1020" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
     <r>
       <t xml:space="preserve">ITEM </t>
@@ -77,7 +77,7 @@
     <t>LAS-01-0002</t>
   </si>
   <si>
-    <t>PIVOT ARM</t>
+    <t>LAS AZIMUTH PIVOT ARM</t>
   </si>
   <si>
     <t>LAS-01-0008</t>
@@ -113,13 +113,19 @@
     <t>LAS-02-0002</t>
   </si>
   <si>
-    <t>LOWER PIVOT HANGER</t>
+    <t>LAS AZIMUTH AXIS - ENCODER</t>
+  </si>
+  <si>
+    <t>LAS-02-0003</t>
+  </si>
+  <si>
+    <t>LAS AZIMUTH AXIS - PASSIVE</t>
   </si>
   <si>
     <t>LAS-02-0006</t>
   </si>
   <si>
-    <t>UPPER PIVOT</t>
+    <t>LAS ELEVATION PIVOT ARM</t>
   </si>
   <si>
     <t>LAS-03-0002</t>
@@ -344,8 +350,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{3319DF4E-E0FC-4595-9133-A3EAD6290C85}">
-  <header guid="{3319DF4E-E0FC-4595-9133-A3EAD6290C85}" dateTime="2020-09-25T11:37:13" maxSheetId="2" userName="andre" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{CFDEBFE4-DDBF-4842-A5B4-8C8C0B1DAF2B}">
+  <header guid="{CFDEBFE4-DDBF-4842-A5B4-8C8C0B1DAF2B}" dateTime="2020-09-29T19:52:52" maxSheetId="2" userName="andre" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -358,7 +364,9 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{CFDEBFE4-DDBF-4842-A5B4-8C8C0B1DAF2B}" name="andre" id="-946593023" dateTime="2020-09-29T20:13:27"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -657,8 +665,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD2C9BD-430A-4F0E-87F1-15EC7B893BC0}">
-  <dimension ref="A1:E29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A963E3-C40E-49A9-855B-850CCD8AFD89}">
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -789,7 +797,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -868,7 +876,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -879,27 +887,25 @@
         <v>30</v>
       </c>
       <c r="D14" s="1">
-        <v>2</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D15" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -913,10 +919,10 @@
         <v>35</v>
       </c>
       <c r="D16" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -930,10 +936,10 @@
         <v>37</v>
       </c>
       <c r="D17" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -947,10 +953,10 @@
         <v>39</v>
       </c>
       <c r="D18" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -964,10 +970,10 @@
         <v>41</v>
       </c>
       <c r="D19" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -984,14 +990,14 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1001,24 +1007,24 @@
         <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D22" s="1">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -1032,10 +1038,10 @@
         <v>49</v>
       </c>
       <c r="D23" s="1">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -1052,7 +1058,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -1069,7 +1075,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -1086,7 +1092,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
@@ -1100,13 +1106,13 @@
         <v>57</v>
       </c>
       <c r="D27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1117,10 +1123,10 @@
         <v>59</v>
       </c>
       <c r="D28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30.75" x14ac:dyDescent="0.25">
@@ -1128,21 +1134,38 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="1">
-        <v>2</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>60</v>
+    </row>
+    <row r="30" spans="1:5" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9D63CC60-58DB-454E-9D11-4AC495F4C5E2}">
+    <customSheetView guid="{638AF512-54A5-44A6-8E4F-2CB6AF9DF51F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>

</xml_diff>

<commit_message>
Added experimental scale kite - Added Dillon's first cut at tow test assy - AA
</commit_message>
<xml_diff>
--- a/solidworks/Line Angle Sensor/LAS BOM.xlsx
+++ b/solidworks/Line Angle Sensor/LAS BOM.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\KiteCAD\kiteCADRepo\solidworks\Line Angle Sensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC84DCA6-42D6-4220-9517-FB5CC55A1E87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F1A46AC-F433-4265-AE99-DBDE0AB1B54A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="28770" windowHeight="15300" xr2:uid="{57B7DC1C-58AE-4505-9A04-94FF693A4A73}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="12795" windowHeight="6795" xr2:uid="{57B7DC1C-58AE-4505-9A04-94FF693A4A73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
-    <customWorkbookView name="andre - Personal View" guid="{638AF512-54A5-44A6-8E4F-2CB6AF9DF51F}" mergeInterval="0" personalView="1" xWindow="1" windowWidth="1918" windowHeight="1020" activeSheetId="1"/>
+    <customWorkbookView name="andre - Personal View" guid="{638AF512-54A5-44A6-8E4F-2CB6AF9DF51F}" mergeInterval="0" personalView="1" xWindow="1" windowWidth="853" windowHeight="453" activeSheetId="1"/>
   </customWorkbookViews>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
   <si>
     <r>
       <t xml:space="preserve">ITEM </t>
@@ -272,6 +274,27 @@
   </si>
   <si>
     <t>RMA MAGNETIC ACTUATOR</t>
+  </si>
+  <si>
+    <t>Flow Speed [m/s]</t>
+  </si>
+  <si>
+    <t>10:1 Tether Ratio</t>
+  </si>
+  <si>
+    <t>50:1 Tether Ratio</t>
+  </si>
+  <si>
+    <t>130 kN</t>
+  </si>
+  <si>
+    <t>490 kN</t>
+  </si>
+  <si>
+    <t>247 kN</t>
+  </si>
+  <si>
+    <t>840 kN</t>
   </si>
 </sst>
 </file>
@@ -350,10 +373,22 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{CFDEBFE4-DDBF-4842-A5B4-8C8C0B1DAF2B}">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1DC38CD7-086F-4183-8666-E9F240615637}" diskRevisions="1" revisionId="30" version="2">
   <header guid="{CFDEBFE4-DDBF-4842-A5B4-8C8C0B1DAF2B}" dateTime="2020-09-29T19:52:52" maxSheetId="2" userName="andre" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{F89CBF4C-1742-4587-85CA-579FBBBD6D1F}" dateTime="2020-09-30T08:10:55" maxSheetId="3" userName="andre" r:id="rId2" minRId="1" maxRId="30">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{1DC38CD7-086F-4183-8666-E9F240615637}" dateTime="2020-10-05T12:03:02" maxSheetId="3" userName="andre" r:id="rId3">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
     </sheetIdMap>
   </header>
 </headers>
@@ -363,10 +398,225 @@
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
 </file>
 
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <ris rId="1" sheetId="2" name="[LAS BOM.xlsx]Sheet2" sheetPosition="1"/>
+  <rcc rId="2" sId="2">
+    <nc r="B1" t="inlineStr">
+      <is>
+        <t>Flow Speed</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="3" sheetId="2" source="B1" destination="A3" sourceSheetId="2"/>
+  <rcc rId="4" sId="2" odxf="1" dxf="1" numFmtId="25">
+    <nc r="B2">
+      <v>0.20902777777777778</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="25" formatCode="h:mm"/>
+    </ndxf>
+  </rcc>
+  <rrc rId="5" sId="2" eol="1" ref="A4:XFD4" action="insertRow"/>
+  <rcc rId="6" sId="2">
+    <nc r="A4">
+      <v>1</v>
+    </nc>
+  </rcc>
+  <rcc rId="7" sId="2">
+    <oc r="A3" t="inlineStr">
+      <is>
+        <t>Flow Speed</t>
+      </is>
+    </oc>
+    <nc r="A3" t="inlineStr">
+      <is>
+        <t>Flow Speed [m/s]</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="8" sId="2" eol="1" ref="A5:XFD5" action="insertRow"/>
+  <rcc rId="9" sId="2">
+    <nc r="A5">
+      <v>2</v>
+    </nc>
+  </rcc>
+  <rcc rId="10" sId="2">
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>5:1 Tether Ratio</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="11" sId="2">
+    <nc r="C3" t="inlineStr">
+      <is>
+        <t>50: Tether Ratio</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="12" sId="2">
+    <oc r="C3" t="inlineStr">
+      <is>
+        <t>50: Tether Ratio</t>
+      </is>
+    </oc>
+    <nc r="C3" t="inlineStr">
+      <is>
+        <t>10:1 Tether Ratio</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="13" sId="2">
+    <nc r="D3" t="inlineStr">
+      <is>
+        <t>50:1 Tether Ratio</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="14" sId="2" numFmtId="25">
+    <oc r="B2">
+      <v>0.20902777777777778</v>
+    </oc>
+    <nc r="B2"/>
+  </rcc>
+  <rcc rId="15" sId="2">
+    <nc r="D4" t="inlineStr">
+      <is>
+        <t>130 kN</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="16" sId="2">
+    <nc r="D5" t="inlineStr">
+      <is>
+        <t>490 kN</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="17" sId="2">
+    <nc r="B5" t="inlineStr">
+      <is>
+        <t>1179 kN</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="18" sId="2">
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>217kN</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="19" sId="2">
+    <oc r="B4" t="inlineStr">
+      <is>
+        <t>217kN</t>
+      </is>
+    </oc>
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>217 kN</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="20" sId="2">
+    <nc r="C4" t="inlineStr">
+      <is>
+        <t>247 kN</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="21" sId="2">
+    <nc r="C5" t="inlineStr">
+      <is>
+        <t>840 kN</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="22" sId="2">
+    <oc r="B4" t="inlineStr">
+      <is>
+        <t>217 kN</t>
+      </is>
+    </oc>
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>X</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="23" sId="2" ref="C1:C1048576" action="insertCol"/>
+  <rcc rId="24" sId="2">
+    <nc r="C3" t="inlineStr">
+      <is>
+        <t>6.25:1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="25" sId="2">
+    <oc r="B3" t="inlineStr">
+      <is>
+        <t>5:1 Tether Ratio</t>
+      </is>
+    </oc>
+    <nc r="B3"/>
+  </rcc>
+  <rcc rId="26" sId="2">
+    <oc r="C3" t="inlineStr">
+      <is>
+        <t>6.25:1</t>
+      </is>
+    </oc>
+    <nc r="C3"/>
+  </rcc>
+  <rcc rId="27" sId="2">
+    <oc r="B4" t="inlineStr">
+      <is>
+        <t>X</t>
+      </is>
+    </oc>
+    <nc r="B4"/>
+  </rcc>
+  <rcc rId="28" sId="2">
+    <oc r="B5" t="inlineStr">
+      <is>
+        <t>1179 kN</t>
+      </is>
+    </oc>
+    <nc r="B5"/>
+  </rcc>
+  <rrc rId="29" sId="2" ref="B1:B1048576" action="deleteCol">
+    <rfmt sheetId="2" sqref="B2" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="25" formatCode="h:mm"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" xfDxf="1" sqref="B1:B1048576" start="0" length="0"/>
+  </rrc>
+  <rrc rId="30" sId="2" ref="B1:B1048576" action="deleteCol">
+    <rfmt sheetId="2" sqref="B2" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="25" formatCode="h:mm"/>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="2" xfDxf="1" sqref="B1:B1048576" start="0" length="0"/>
+  </rrc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{638AF512-54A5-44A6-8E4F-2CB6AF9DF51F}" action="delete"/>
+  <rcv guid="{638AF512-54A5-44A6-8E4F-2CB6AF9DF51F}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{CFDEBFE4-DDBF-4842-A5B4-8C8C0B1DAF2B}" name="andre" id="-946593023" dateTime="2020-09-29T20:13:27"/>
-</users>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -668,7 +918,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A963E3-C40E-49A9-855B-850CCD8AFD89}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:D28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1165,7 +1417,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{638AF512-54A5-44A6-8E4F-2CB6AF9DF51F}">
+    <customSheetView guid="{638AF512-54A5-44A6-8E4F-2CB6AF9DF51F}" topLeftCell="A23">
+      <selection activeCell="B15" sqref="B15:D28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -1173,4 +1426,62 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCBDDDE-BF34-4EEC-BDD4-93533CA4C7AB}">
+  <dimension ref="A3:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C13:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{638AF512-54A5-44A6-8E4F-2CB6AF9DF51F}">
+      <selection activeCell="C14" sqref="C13:C14"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>